<commit_message>
Backup QR Scanner data - 2026-01-02T17:47:46.401Z - Cache Bust: 1767376066401
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Rheumatology_scanner1767091486285_406fb96fa39b42283255a033ca2f67cc312ec0c094804fa24386df6c77fc94cd.xlsx
+++ b/log_history/Y5_B2526_Rheumatology_scanner1767091486285_406fb96fa39b42283255a033ca2f67cc312ec0c094804fa24386df6c77fc94cd.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Rheumatology" sheetId="1" r:id="rId1"/>
+    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,189 +442,9 @@
         <v>tasneemahmoud@gmail.com</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>200536</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C3" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>12:45:06</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F3" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>200840</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C4" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>12:45:12</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F4" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>200560</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C5" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>12:45:21</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F5" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>200770</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C6" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>12:45:36</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F6" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>200673</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C7" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D7" t="str">
-        <v>12:45:46</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F7" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>200957</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C8" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D8" t="str">
-        <v>12:45:53</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F8" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>200660</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C9" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D9" t="str">
-        <v>12:46:00</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F9" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>200554</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C10" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D10" t="str">
-        <v>12:46:18</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F10" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>200620</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Rheumatology</v>
-      </c>
-      <c r="C11" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D11" t="str">
-        <v>12:46:33</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F11" t="str">
-        <v>tasneemahmoud@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>